<commit_message>
Added the lumpy demand items. Pending analysis
</commit_message>
<xml_diff>
--- a/bip8013_data.xlsx
+++ b/bip8013_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2506\Desktop\TESIS\DOCUMENTOS TESIS\Capitulos\R\Tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Esteban\TESIS\Tesis\Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD8152D-0916-46B5-BCC2-1645016D7CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,18 @@
     <sheet name="Optimal" sheetId="9" r:id="rId5"/>
     <sheet name="interdemand inter." sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -359,7 +371,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
@@ -425,6 +437,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -434,11 +447,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -456,7 +468,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -493,7 +505,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -519,7 +530,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1089,7 +1100,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547302112"/>
@@ -1134,7 +1145,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="547309328"/>
@@ -1151,7 +1162,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1177,7 +1187,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1207,7 +1217,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1221,7 +1231,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1233,7 +1243,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1259,7 +1268,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2668,7 +2677,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="641603752"/>
@@ -2727,7 +2736,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="641603424"/>
@@ -2744,7 +2753,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2770,7 +2778,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2800,7 +2808,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2814,7 +2822,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2826,7 +2834,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2852,7 +2859,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4258,7 +4265,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="677836616"/>
@@ -4317,7 +4324,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="677839240"/>
@@ -4334,7 +4341,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4360,7 +4366,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4390,7 +4396,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4404,7 +4410,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4416,7 +4422,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4442,7 +4447,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5848,7 +5853,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="630319192"/>
@@ -5907,7 +5912,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="630314928"/>
@@ -5924,7 +5929,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5950,7 +5954,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5980,7 +5984,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5994,7 +5998,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6006,7 +6010,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6032,7 +6035,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7438,7 +7441,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="448300120"/>
@@ -7497,7 +7500,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="448307336"/>
@@ -7514,7 +7517,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7540,7 +7542,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7570,7 +7572,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10313,7 +10315,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10348,7 +10356,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10385,7 +10399,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10422,7 +10442,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10459,7 +10485,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10480,7 +10512,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10555,6 +10587,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -10590,6 +10639,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10765,22 +10831,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E33" sqref="E32:E33"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="3" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10788,7 +10854,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -10802,7 +10868,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -10834,7 +10900,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -10872,7 +10938,7 @@
         <v>318.20479999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -10910,7 +10976,7 @@
         <v>758.51610000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -10948,7 +11014,7 @@
         <v>1277.1859999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -10994,29 +11060,29 @@
         <v>518.66989999999987</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="R8" s="8" t="s">
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="R8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -11056,7 +11122,7 @@
         <v>1.9161422063818451E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -11096,7 +11162,7 @@
         <v>6.9105048129257493E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -11136,7 +11202,7 @@
         <v>5.3868426368602689E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -11176,29 +11242,29 @@
       </c>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="R13" s="9" t="s">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="R13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -11238,7 +11304,7 @@
         <v>-5.057638196473418E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -11278,7 +11344,7 @@
         <v>2.0711491819355088E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -11318,7 +11384,7 @@
         <v>1.6439993824779938E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -11358,7 +11424,7 @@
       </c>
       <c r="V17" s="4"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -11374,7 +11440,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -11387,7 +11453,7 @@
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -11419,7 +11485,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -11454,7 +11520,7 @@
         <v>0.16236999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -11492,7 +11558,7 @@
         <v>333.1003</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -11530,7 +11596,7 @@
         <v>756.7885</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -11572,20 +11638,20 @@
         <v>1322.5387000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
       <c r="R25" t="s">
         <v>58</v>
       </c>
@@ -11606,7 +11672,7 @@
         <v>565.75020000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -11629,15 +11695,15 @@
         <f>(L23-O23)/O23</f>
         <v>4.9269311128286093E-2</v>
       </c>
-      <c r="R26" s="8" t="s">
+      <c r="R26" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -11680,7 +11746,7 @@
         <v>2.2142382773296616E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -11715,15 +11781,15 @@
         <v>1.7219967691875039E-2</v>
       </c>
       <c r="U28" s="5">
-        <f t="shared" ref="T28:V28" si="0">($S$24-U6)/U6</f>
+        <f>($S$24-U6)/U6</f>
         <v>1.7868087088026674E-2</v>
       </c>
       <c r="V28" s="5">
-        <f t="shared" si="0"/>
+        <f>($S$24-V6)/V6</f>
         <v>1.7922918040128927E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -11766,20 +11832,20 @@
         <v>3.7317075836198567E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
       <c r="R30" s="4" t="s">
         <v>102</v>
       </c>
@@ -11792,15 +11858,15 @@
         <v>3.23215827382035E-2</v>
       </c>
       <c r="U30" s="5">
-        <f t="shared" ref="T30:V30" si="1">($T$24-U6)/U6</f>
+        <f>($T$24-U6)/U6</f>
         <v>3.2979324094143198E-2</v>
       </c>
       <c r="V30" s="5">
-        <f t="shared" si="1"/>
+        <f>($T$24-V6)/V6</f>
         <v>3.3034969064803452E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -11835,15 +11901,15 @@
         <v>3.7113287821255746E-2</v>
       </c>
       <c r="U31" s="5">
-        <f t="shared" ref="T31:V31" si="2">($U$24-N6)/N6</f>
+        <f t="shared" ref="U31:V31" si="0">($U$24-N6)/N6</f>
         <v>3.7496108306995637E-2</v>
       </c>
       <c r="V31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.7517561136419887E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -11886,7 +11952,7 @@
         <v>3.3234626749745276E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -11917,19 +11983,19 @@
         <v>7.7859761445562108E-3</v>
       </c>
       <c r="T33" s="5">
-        <f t="shared" ref="T33:V33" si="3">($V$24-M6)/M6</f>
+        <f t="shared" ref="T33:V33" si="1">($V$24-M6)/M6</f>
         <v>3.9397065174379853E-2</v>
       </c>
       <c r="U33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3.9780728650722526E-2</v>
       </c>
       <c r="V33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3.9802228720391956E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -11960,34 +12026,34 @@
         <v>1.6041071288502975E-2</v>
       </c>
       <c r="T34" s="5">
-        <f t="shared" ref="T34:V34" si="4">($V$24-T6)/T6</f>
+        <f t="shared" ref="T34:V34" si="2">($V$24-T6)/T6</f>
         <v>3.4794767667400639E-2</v>
       </c>
       <c r="U34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3.5454084807510715E-2</v>
       </c>
       <c r="V34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3.5509863089636232E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="R35" s="9" t="s">
+      <c r="R35" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -12002,19 +12068,19 @@
         <v>-9.5288746013062944E-3</v>
       </c>
       <c r="T36" s="5">
-        <f t="shared" ref="T36:V36" si="5">($S$23-M5)/M5</f>
+        <f t="shared" ref="T36:V36" si="3">($S$23-M5)/M5</f>
         <v>-6.6420607665871653E-3</v>
       </c>
       <c r="U36" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>-5.7328376799518693E-3</v>
       </c>
       <c r="V36" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>-5.6827512237483495E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -12033,15 +12099,15 @@
         <v>-1.06057582085E-2</v>
       </c>
       <c r="U37" s="5">
-        <f t="shared" ref="T37:V37" si="6">($S$23-U5)/U5</f>
+        <f t="shared" ref="U37:V37" si="4">($S$23-U5)/U5</f>
         <v>-8.7195415801523055E-3</v>
       </c>
       <c r="V37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-8.5565751340018325E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -12053,19 +12119,19 @@
         <v>-6.1416322483173243E-3</v>
       </c>
       <c r="T38" s="5">
-        <f t="shared" ref="T38:V38" si="7">($T$23-M5)/M5</f>
+        <f t="shared" ref="T38:V38" si="5">($T$23-M5)/M5</f>
         <v>-3.244946002545102E-3</v>
       </c>
       <c r="U38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.332613527994912E-3</v>
       </c>
       <c r="V38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.2823557846519556E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -12077,19 +12143,19 @@
         <v>-1.0892036596175415E-4</v>
       </c>
       <c r="T39" s="5">
-        <f t="shared" ref="T39:V39" si="8">($T$23-T5)/T5</f>
+        <f t="shared" ref="T39:V39" si="6">($T$23-T5)/T5</f>
         <v>-7.2221986138166373E-3</v>
       </c>
       <c r="U39" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-5.3295314462390581E-3</v>
       </c>
       <c r="V39" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-5.1660076826319104E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -12105,15 +12171,15 @@
         <v>-3.4619714149924877E-3</v>
       </c>
       <c r="U40" s="5">
-        <f t="shared" ref="T40:V40" si="9">($U$23-N5)/N5</f>
+        <f t="shared" ref="U40:V40" si="7">($U$23-N5)/N5</f>
         <v>-2.5498375843626712E-3</v>
       </c>
       <c r="V40" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>-2.4995907837357155E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -12125,19 +12191,19 @@
         <v>-3.2662859135751225E-4</v>
       </c>
       <c r="T41" s="5">
-        <f t="shared" ref="T41:V41" si="10">($U$23-T5)/T5</f>
+        <f t="shared" ref="T41:V41" si="8">($U$23-T5)/T5</f>
         <v>-7.4383580513337662E-3</v>
       </c>
       <c r="U41" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-5.5461029778519451E-3</v>
       </c>
       <c r="V41" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-5.38261481859122E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -12149,19 +12215,19 @@
         <v>-3.2560621141065819E-3</v>
       </c>
       <c r="T42" s="5">
-        <f t="shared" ref="T42:V42" si="11">($V$23-M5)/M5</f>
+        <f t="shared" ref="T42:V42" si="9">($V$23-M5)/M5</f>
         <v>-3.5096562438995517E-4</v>
       </c>
       <c r="U42" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5.6401571787263163E-4</v>
       </c>
       <c r="V42" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>6.1441937963606786E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="R43" s="4" t="s">
         <v>106</v>
       </c>
@@ -12170,20 +12236,20 @@
         <v>2.7941651545463375E-3</v>
       </c>
       <c r="T43" s="5">
-        <f t="shared" ref="T43:V43" si="12">($V$23-T5)/T5</f>
+        <f t="shared" ref="T43:V43" si="10">($V$23-T5)/T5</f>
         <v>-4.3397657978933796E-3</v>
       </c>
       <c r="U43" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-2.441603457130191E-3</v>
       </c>
       <c r="V43" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-2.2776049183399695E-3</v>
       </c>
     </row>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K25:O25"/>
@@ -12202,24 +12268,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12251,7 +12317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -12274,7 +12340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -12297,7 +12363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -12320,7 +12386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -12343,7 +12409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -12366,7 +12432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -12389,7 +12455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -12412,7 +12478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -12435,7 +12501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -12458,7 +12524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -12481,7 +12547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -12504,7 +12570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -12527,7 +12593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -12559,7 +12625,7 @@
         <v>5479.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -12591,7 +12657,7 @@
         <v>-548.45000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -12623,7 +12689,7 @@
         <v>-493.60500000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -12655,7 +12721,7 @@
         <v>-444.24450000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -12687,7 +12753,7 @@
         <v>1120.17995</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -12719,7 +12785,7 @@
         <v>2489.161955</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -12751,7 +12817,7 @@
         <v>240.24575949999991</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -12783,7 +12849,7 @@
         <v>2215.2211835500002</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -12815,7 +12881,7 @@
         <v>1993.699065195</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -12847,7 +12913,7 @@
         <v>794.32915867549991</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -12879,7 +12945,7 @@
         <v>714.89624280794987</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -12911,7 +12977,7 @@
         <v>-1356.5933814728451</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -12943,7 +13009,7 @@
         <v>-1220.9340433255611</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -12975,7 +13041,7 @@
         <v>-98.840638993004632</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -13007,7 +13073,7 @@
         <v>-88.956575093704032</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -13051,7 +13117,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -13098,7 +13164,7 @@
         <v>303.51330000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -13145,7 +13211,7 @@
         <v>756.32380000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -13192,7 +13258,7 @@
         <v>1271.9137000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -13243,7 +13309,7 @@
         <v>515.58990000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -13274,15 +13340,15 @@
       <c r="J34">
         <v>296.52482877562659</v>
       </c>
-      <c r="N34" s="8" t="s">
+      <c r="N34" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -13330,7 +13396,7 @@
         <v>3.1768900673056551E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -13378,7 +13444,7 @@
         <v>3.898063209791021E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -13426,7 +13492,7 @@
         <v>2.0677503513007207E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>804.45010000000002</v>
       </c>
@@ -13456,7 +13522,7 @@
       </c>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39">
         <f>SUM(B13:B37)/15</f>
         <v>1867.2</v>
@@ -13473,15 +13539,15 @@
       <c r="F39">
         <v>755.99332939270596</v>
       </c>
-      <c r="N39" s="9" t="s">
+      <c r="N39" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>804.45010000000002</v>
       </c>
@@ -13511,7 +13577,7 @@
         <v>3.8831251905599652E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>804.45010000000002</v>
       </c>
@@ -13541,7 +13607,7 @@
         <v>9.6572393993158941E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>804.45010000000002</v>
       </c>
@@ -13571,7 +13637,7 @@
         <v>5.0375249331021729E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N43" s="4" t="s">
         <v>52</v>
       </c>
@@ -13600,25 +13666,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13650,7 +13716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -13673,7 +13739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -13696,7 +13762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -13719,7 +13785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -13742,7 +13808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -13765,7 +13831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -13788,7 +13854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -13811,7 +13877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -13834,7 +13900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -13857,7 +13923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -13880,7 +13946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -13903,7 +13969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -13926,7 +13992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -13958,7 +14024,7 @@
         <v>5479.25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -13990,7 +14056,7 @@
         <v>-822.63750000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -14022,7 +14088,7 @@
         <v>-699.24187500000005</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -14054,7 +14120,7 @@
         <v>-594.35559375000003</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -14086,7 +14152,7 @@
         <v>1014.7977453125</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -14118,7 +14184,7 @@
         <v>2343.5780835156252</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -14150,7 +14216,7 @@
         <v>-7.9586290117188128</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -14182,7 +14248,7 @@
         <v>1992.235165340039</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -14214,7 +14280,7 @@
         <v>1693.3998905390331</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -14246,7 +14312,7 @@
         <v>439.38990695817819</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -14278,7 +14344,7 @@
         <v>373.48142091445152</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -14310,7 +14376,7 @@
         <v>-1682.5407922227159</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -14342,7 +14408,7 @@
         <v>-1430.1596733893091</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -14374,7 +14440,7 @@
         <v>-215.63572238091231</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -14406,7 +14472,7 @@
         <v>-183.29036402377551</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -14438,7 +14504,7 @@
         <v>-155.7968094202092</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -14482,7 +14548,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -14529,7 +14595,7 @@
         <v>318.20479999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -14576,7 +14642,7 @@
         <v>758.51610000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -14623,7 +14689,7 @@
         <v>1277.1859999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -14674,7 +14740,7 @@
         <v>518.66989999999987</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -14705,15 +14771,15 @@
       <c r="J35">
         <v>-652.59150370875227</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -14761,7 +14827,7 @@
         <v>1.9161422063818451E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -14809,7 +14875,7 @@
         <v>6.9105048129257493E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>783.27279999999996</v>
       </c>
@@ -14839,7 +14905,7 @@
         <v>5.3868426368602689E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>783.27279999999996</v>
       </c>
@@ -14869,7 +14935,7 @@
       </c>
       <c r="Q39" s="4"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>783.27279999999996</v>
       </c>
@@ -14882,15 +14948,15 @@
       <c r="F40">
         <v>730.98243670120416</v>
       </c>
-      <c r="M40" s="9" t="s">
+      <c r="M40" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>783.27279999999996</v>
       </c>
@@ -14920,7 +14986,7 @@
         <v>-5.057638196473418E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>783.27279999999996</v>
       </c>
@@ -14950,7 +15016,7 @@
         <v>2.0711491819355088E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M43" s="4" t="s">
         <v>51</v>
       </c>
@@ -14968,7 +15034,7 @@
         <v>1.6439993824779938E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M44" s="4" t="s">
         <v>52</v>
       </c>
@@ -14997,25 +15063,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15047,7 +15113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -15070,7 +15136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -15093,7 +15159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -15116,7 +15182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -15139,7 +15205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -15162,7 +15228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -15185,7 +15251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -15208,7 +15274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -15231,7 +15297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -15254,7 +15320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -15277,7 +15343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -15300,7 +15366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -15323,7 +15389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -15355,7 +15421,7 @@
         <v>5477.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -15387,7 +15453,7 @@
         <v>-2741.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -15419,7 +15485,7 @@
         <v>-1370.625</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -15451,7 +15517,7 @@
         <v>-685.3125</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -15483,7 +15549,7 @@
         <v>1177.34375</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -15515,7 +15581,7 @@
         <v>2069.671875</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -15547,7 +15613,7 @@
         <v>-965.1640625</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -15579,7 +15645,7 @@
         <v>1516.41796875</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -15611,7 +15677,7 @@
         <v>758.208984375</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -15643,7 +15709,7 @@
         <v>-620.8955078125</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -15675,7 +15741,7 @@
         <v>-310.44775390625</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -15707,7 +15773,7 @@
         <v>-2155.223876953125</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -15739,7 +15805,7 @@
         <v>-1077.611938476563</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -15771,7 +15837,7 @@
         <v>461.19403076171881</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -15803,7 +15869,7 @@
         <v>230.5970153808594</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -15835,7 +15901,7 @@
         <v>115.2985076904297</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -15867,7 +15933,7 @@
         <v>-942.35074615478516</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -15899,7 +15965,7 @@
         <v>-471.17537307739258</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -15931,7 +15997,7 @@
         <v>-235.58768653869629</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -15975,7 +16041,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -16022,7 +16088,7 @@
         <v>329.14150000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -16069,7 +16135,7 @@
         <v>754.19240000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -16116,7 +16182,7 @@
         <v>1313.6713</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -16167,7 +16233,7 @@
         <v>559.47889999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>816.21230000000003</v>
       </c>
@@ -16180,15 +16246,15 @@
       <c r="F38">
         <v>661.88229640603311</v>
       </c>
-      <c r="L38" s="8" t="s">
+      <c r="L38" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>816.21230000000003</v>
       </c>
@@ -16218,7 +16284,7 @@
         <v>4.9269311128286093E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>816.21230000000003</v>
       </c>
@@ -16248,7 +16314,7 @@
         <v>3.3351569757214081E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>816.21230000000003</v>
       </c>
@@ -16278,7 +16344,7 @@
         <v>4.4820192083057193E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>816.21230000000003</v>
       </c>
@@ -16308,16 +16374,16 @@
       </c>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L43" s="9" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L43" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L44" s="4" t="s">
         <v>49</v>
       </c>
@@ -16335,7 +16401,7 @@
         <v>8.0683098901553396E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L45" s="4" t="s">
         <v>50</v>
       </c>
@@ -16353,7 +16419,7 @@
         <v>4.2165235290093091E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L46" s="4" t="s">
         <v>51</v>
       </c>
@@ -16371,7 +16437,7 @@
         <v>7.0805539806553432E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L47" s="4" t="s">
         <v>52</v>
       </c>
@@ -16400,25 +16466,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="L30" sqref="L30:P45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16450,7 +16516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -16473,7 +16539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -16496,7 +16562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -16519,7 +16585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -16542,7 +16608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -16565,7 +16631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -16588,7 +16654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -16611,7 +16677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -16634,7 +16700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -16657,7 +16723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -16680,7 +16746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -16703,7 +16769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -16726,7 +16792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -16758,7 +16824,7 @@
         <v>5479.0863582265229</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -16790,7 +16856,7 @@
         <v>-1002.098077246603</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -16822,7 +16888,7 @@
         <v>-818.98634434783776</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -16854,7 +16920,7 @@
         <v>-669.33431712709989</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -16886,7 +16952,7 @@
         <v>972.97204138275083</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -16918,7 +16984,7 @@
         <v>2276.1824610961889</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -16950,7 +17016,7 @@
         <v>-139.7406150066036</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -16982,7 +17048,7 @@
         <v>1884.793957657686</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -17014,7 +17080,7 @@
         <v>1540.3886588349339</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -17046,7 +17112,7 @@
         <v>258.9159736144652</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -17078,7 +17144,7 @@
         <v>211.60468375151851</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -17110,7 +17176,7 @@
         <v>-1827.061491956252</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -17142,7 +17208,7 @@
         <v>-1493.205551603636</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -17174,7 +17240,7 @@
         <v>-220.35455793696181</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -17206,7 +17272,7 @@
         <v>-180.08953211549331</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -17238,7 +17304,7 @@
         <v>-147.1820682141522</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -17282,7 +17348,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -17326,7 +17392,7 @@
         <v>0.16236999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -17373,7 +17439,7 @@
         <v>333.1003</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -17420,7 +17486,7 @@
         <v>756.7885</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -17467,7 +17533,7 @@
         <v>1322.5387000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -17518,7 +17584,7 @@
         <v>565.75020000000006</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -17549,15 +17615,15 @@
       <c r="J36">
         <v>2516.7070889100542</v>
       </c>
-      <c r="L36" s="8" t="s">
+      <c r="L36" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -17605,7 +17671,7 @@
         <v>-1.6983850831737504E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>770.82339999999999</v>
       </c>
@@ -17635,7 +17701,7 @@
         <v>-2.3900245792429992E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>770.82339999999999</v>
       </c>
@@ -17665,7 +17731,7 @@
         <v>-2.1972135862640347E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>770.82339999999999</v>
       </c>
@@ -17695,7 +17761,7 @@
       </c>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>770.82339999999999</v>
       </c>
@@ -17708,15 +17774,15 @@
       <c r="F41">
         <v>811.97969712959537</v>
       </c>
-      <c r="L41" s="9" t="s">
+      <c r="L41" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>770.82339999999999</v>
       </c>
@@ -17746,7 +17812,7 @@
         <v>-6.2933038755213578E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L43" s="4" t="s">
         <v>50</v>
       </c>
@@ -17764,7 +17830,7 @@
         <v>-2.8949964223821349E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L44" s="4" t="s">
         <v>51</v>
       </c>
@@ -17782,7 +17848,7 @@
         <v>-3.1120980300308053E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L45" s="4" t="s">
         <v>52</v>
       </c>
@@ -17811,49 +17877,49 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:AG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" customWidth="1"/>
+    <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="C1" s="10">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C1" s="11">
         <v>0.1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11">
         <v>0.15</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11">
         <v>0.5</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-    </row>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>108</v>
       </c>
@@ -17900,7 +17966,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <v>44912</v>
       </c>
@@ -17936,7 +18002,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B4" s="6">
         <v>44579</v>
       </c>
@@ -17972,7 +18038,7 @@
         <v>0.29000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>44610</v>
       </c>
@@ -18009,7 +18075,7 @@
         <v>0.36100000000000004</v>
       </c>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>44638</v>
       </c>
@@ -18053,7 +18119,7 @@
         <v>1.6500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>44669</v>
       </c>
@@ -18090,7 +18156,7 @@
         <v>0.48241000000000006</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>44699</v>
       </c>
@@ -18127,7 +18193,7 @@
         <v>0.53416900000000012</v>
       </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>44730</v>
       </c>
@@ -18164,7 +18230,7 @@
         <v>0.5807521000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B10" s="6">
         <v>44760</v>
       </c>
@@ -18208,7 +18274,7 @@
         <v>0.62267689000000015</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>44791</v>
       </c>
@@ -18248,7 +18314,7 @@
         <v>0.66040920100000011</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>44822</v>
       </c>
@@ -18288,7 +18354,7 @@
         <v>0.69436828090000013</v>
       </c>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>44852</v>
       </c>
@@ -18330,7 +18396,7 @@
         <v>0.72493145281000015</v>
       </c>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B14" s="6">
         <v>44883</v>
       </c>
@@ -18370,7 +18436,7 @@
         <v>0.75243830752900009</v>
       </c>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>44913</v>
       </c>
@@ -18410,7 +18476,7 @@
       <c r="N15" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q15" s="11">
+      <c r="Q15" s="8">
         <v>1</v>
       </c>
       <c r="V15">
@@ -18434,7 +18500,7 @@
         <v>0.7771944767761001</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B16" s="6">
         <v>44580</v>
       </c>
@@ -18474,7 +18540,7 @@
       <c r="N16" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q16" s="11">
+      <c r="Q16" s="8">
         <v>1</v>
       </c>
       <c r="V16">
@@ -18498,7 +18564,7 @@
         <v>0.79947502909849011</v>
       </c>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>44611</v>
       </c>
@@ -18538,7 +18604,7 @@
       <c r="N17" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="8">
         <v>1</v>
       </c>
       <c r="V17">
@@ -18562,7 +18628,7 @@
         <v>0.81952752618864111</v>
       </c>
     </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>44639</v>
       </c>
@@ -18602,7 +18668,7 @@
       <c r="N18" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q18" s="11">
+      <c r="Q18" s="8">
         <v>1</v>
       </c>
       <c r="V18">
@@ -18626,7 +18692,7 @@
         <v>0.83757477356977694</v>
       </c>
     </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>44670</v>
       </c>
@@ -18666,7 +18732,7 @@
       <c r="N19" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q19" s="11">
+      <c r="Q19" s="8">
         <v>3</v>
       </c>
       <c r="V19">
@@ -18690,7 +18756,7 @@
         <v>0.85381729621279923</v>
       </c>
     </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>44700</v>
       </c>
@@ -18730,7 +18796,7 @@
       <c r="N20" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q20" s="11">
+      <c r="Q20" s="8">
         <v>1</v>
       </c>
       <c r="V20">
@@ -18754,7 +18820,7 @@
         <v>0.86843556659151933</v>
       </c>
     </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>44731</v>
       </c>
@@ -18794,7 +18860,7 @@
       <c r="N21" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q21" s="11">
+      <c r="Q21" s="8">
         <v>1</v>
       </c>
       <c r="V21">
@@ -18818,7 +18884,7 @@
         <v>0.88159200993236742</v>
       </c>
     </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>44761</v>
       </c>
@@ -18858,7 +18924,7 @@
       <c r="N22" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q22" s="11">
+      <c r="Q22" s="8">
         <v>4</v>
       </c>
       <c r="V22">
@@ -18882,7 +18948,7 @@
         <v>0.89343280893913068</v>
       </c>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>44792</v>
       </c>
@@ -18922,7 +18988,7 @@
       <c r="N23" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q23" s="11">
+      <c r="Q23" s="8">
         <v>1</v>
       </c>
       <c r="V23">
@@ -18946,7 +19012,7 @@
         <v>0.90408952804521758</v>
       </c>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <v>44823</v>
       </c>
@@ -18986,7 +19052,7 @@
       <c r="N24" s="2">
         <v>1.739206</v>
       </c>
-      <c r="Q24" s="11">
+      <c r="Q24" s="8">
         <v>2</v>
       </c>
       <c r="V24">
@@ -19010,7 +19076,7 @@
         <v>0.91368057524069579</v>
       </c>
     </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <v>44853</v>
       </c>
@@ -19071,7 +19137,7 @@
         <v>0.92231251771662626</v>
       </c>
     </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <v>44884</v>
       </c>
@@ -19132,7 +19198,7 @@
         <v>0.93008126594496365</v>
       </c>
     </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>44914</v>
       </c>
@@ -19193,7 +19259,7 @@
         <v>0.93707313935046732</v>
       </c>
     </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>44581</v>
       </c>
@@ -19254,7 +19320,7 @@
         <v>0.94336582541542058</v>
       </c>
     </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>44612</v>
       </c>
@@ -19315,7 +19381,7 @@
         <v>0.94902924287387846</v>
       </c>
     </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>44640</v>
       </c>
@@ -19376,7 +19442,7 @@
         <v>0.95412631858649066</v>
       </c>
     </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>44671</v>
       </c>
@@ -19437,7 +19503,7 @@
         <v>0.95871368672784163</v>
       </c>
     </row>
-    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>44701</v>
       </c>
@@ -19498,7 +19564,7 @@
         <v>0.96284231805505749</v>
       </c>
     </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>44732</v>
       </c>
@@ -19559,7 +19625,7 @@
         <v>0.96655808624955175</v>
       </c>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>44762</v>
       </c>
@@ -19620,7 +19686,7 @@
         <v>0.96990227762459658</v>
       </c>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B35" s="6">
         <v>44793</v>
       </c>
@@ -19681,7 +19747,7 @@
         <v>0.87291204986213689</v>
       </c>
     </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>44824</v>
       </c>
@@ -19741,7 +19807,7 @@
         <v>0.98562084487592316</v>
       </c>
     </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B37" s="6">
         <v>44854</v>
       </c>
@@ -19801,7 +19867,7 @@
         <v>1.1870587603883309</v>
       </c>
     </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B38" s="6">
         <v>44885</v>
       </c>
@@ -19862,7 +19928,7 @@
         <v>1.1683528843494979</v>
       </c>
     </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:29" x14ac:dyDescent="0.3">
       <c r="W39">
         <v>1</v>
       </c>

</xml_diff>